<commit_message>
Wed May 17 16:05:42 CST 2023
</commit_message>
<xml_diff>
--- a/书籍/古语.xlsx
+++ b/书籍/古语.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>句子</t>
   </si>
@@ -128,6 +128,42 @@
   </si>
   <si>
     <t>追求事情的根本，自律</t>
+  </si>
+  <si>
+    <t>蓬生麻中，不扶而直</t>
+  </si>
+  <si>
+    <t>劝学</t>
+  </si>
+  <si>
+    <t>荀子</t>
+  </si>
+  <si>
+    <t>交友</t>
+  </si>
+  <si>
+    <t>优化自己的成长环境，结交好的朋友</t>
+  </si>
+  <si>
+    <t>君子居易以侍命，小人行险以侥幸。</t>
+  </si>
+  <si>
+    <t>礼记·中庸</t>
+  </si>
+  <si>
+    <t>品德高尚的人安于自己的地位等候天命的到来，无德奸诈的人则冒险求得本不应该获取的东西。</t>
+  </si>
+  <si>
+    <t>君子而和不同，小人同而不和</t>
+  </si>
+  <si>
+    <t>君子可以与他周围保持和谐融洽的氛围，但他对待任何事情都持有自己的独立见解，而不是人云亦云，盲目附和；小人则没有自己独立的见解，虽然常和他人保持一致，但实际并不讲求真正的和谐贯通。</t>
+  </si>
+  <si>
+    <t>如切如磋，如琢如磨</t>
+  </si>
+  <si>
+    <t>诗经·卫风·淇奥</t>
   </si>
 </sst>
 </file>
@@ -136,9 +172,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -159,35 +195,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -202,7 +209,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -210,9 +217,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -225,52 +232,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -278,6 +239,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -286,15 +248,89 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -315,37 +351,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -357,31 +477,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,19 +501,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -417,85 +519,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -524,17 +560,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -543,7 +573,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -563,26 +593,28 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,164 +636,168 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1106,10 +1142,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>
@@ -1118,7 +1156,7 @@
     <col min="2" max="2" width="20.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="1"/>
     <col min="4" max="4" width="12.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="57.8046875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="74.3359375" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1300,20 +1338,20 @@
       <c r="E11" s="3"/>
     </row>
     <row r="12" customHeight="1" spans="1:5">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:5">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1322,11 +1360,68 @@
       <c r="C13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:5">
+      <c r="A14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:5">
+      <c r="A15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" ht="50" customHeight="1" spans="1:5">
+      <c r="A16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mon May 29 10:28:36 CST 2023
</commit_message>
<xml_diff>
--- a/书籍/古语.xlsx
+++ b/书籍/古语.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>句子</t>
   </si>
@@ -164,6 +164,21 @@
   </si>
   <si>
     <t>诗经·卫风·淇奥</t>
+  </si>
+  <si>
+    <t>人的修为没有尽头，永远可以切磋琢磨下去</t>
+  </si>
+  <si>
+    <t>主好要则百事详，主好详则百事荒</t>
+  </si>
+  <si>
+    <t>荀子·王霸</t>
+  </si>
+  <si>
+    <t>管理</t>
+  </si>
+  <si>
+    <t>君主如果喜欢抓住要领，那么很多事情都能理解得很清楚，如果君主什么事情都要弄得很清楚，那么很多事情就容易荒废。</t>
   </si>
 </sst>
 </file>
@@ -1142,12 +1157,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>
@@ -1416,12 +1431,36 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" customHeight="1" spans="1:2">
-      <c r="A17" s="1" t="s">
+    <row r="17" customHeight="1" spans="1:5">
+      <c r="A17" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="4" t="s">
         <v>49</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" customHeight="1" spans="1:5">
+      <c r="A18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>